<commit_message>
Hai hello new changes done by ranjith 01-09-2025
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/zltUI/ZltTestData.xlsx
+++ b/src/test/resources/testdata/zltUI/ZltTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ranjith\Downloads\ZlaataProductionPGR (3)\ZlaataProductionPGR\src\test\resources\testdata\zltUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowthamraj\git\zlaataautomation-pixel\zlaata\zlaata\zlaata\zlaata\src\test\resources\testdata\zltUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD66B2A-C601-4B66-B7CE-DA44B0C215A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D21428C-9EE0-4061-98C8-1385764245E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-Zlaata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5711" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5711" uniqueCount="694">
   <si>
     <t>S.No</t>
   </si>
@@ -2105,6 +2105,9 @@
   </si>
   <si>
     <t>Verify user can login in coupon popup</t>
+  </si>
+  <si>
+    <t>6383041822</t>
   </si>
 </sst>
 </file>
@@ -3537,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75D1F84-2AD1-4552-9C1F-85B59D75CCFA}">
   <dimension ref="A1:Z199"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" zoomScale="109" workbookViewId="0">
-      <selection activeCell="D205" sqref="D205"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10437,8 +10440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74813B-34A6-48F5-8B35-1C10409ED694}">
   <dimension ref="A1:U197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="C204" sqref="C204"/>
+    <sheetView topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20065,7 +20068,7 @@
       </c>
     </row>
     <row r="152" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A152" s="48" t="s">
+      <c r="A152" s="63" t="s">
         <v>510</v>
       </c>
       <c r="B152" s="48" t="s">
@@ -20267,7 +20270,7 @@
         <v>22</v>
       </c>
       <c r="C155" s="36" t="s">
-        <v>575</v>
+        <v>693</v>
       </c>
       <c r="D155" s="48" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Hai pushed code for admin 05-09-2025 17:42
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/zltUI/ZltTestData.xlsx
+++ b/src/test/resources/testdata/zltUI/ZltTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gowthamraj\git\zlaatanew\src\test\resources\testdata\zltUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ranjith\git\zlaataWoking\src\test\resources\testdata\zltUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15995E10-E53C-4A35-8FC4-31702BC990F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727D6848-C8B7-4FFC-8529-949B53539CFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{905F911F-FA1A-4DDD-B945-7467E9458D34}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases-Zlaata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4780" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5145" uniqueCount="614">
   <si>
     <t>S.No</t>
   </si>
@@ -1841,6 +1841,33 @@
   </si>
   <si>
     <t>Verify Accessories, Recently Viewed, and Top Selling buttons on Checkout page</t>
+  </si>
+  <si>
+    <t>Admin Banner upload</t>
+  </si>
+  <si>
+    <t>TC_UI_Zlaata_ADM_01</t>
+  </si>
+  <si>
+    <t>TD_UI_Zlaata_ADM_01</t>
+  </si>
+  <si>
+    <t>Verify banner upload on home page section</t>
+  </si>
+  <si>
+    <t>https://qa.adm.testingserver8.com/admin/home-page-banner</t>
+  </si>
+  <si>
+    <t>Banner Tiltle</t>
+  </si>
+  <si>
+    <t>Home Page Automation</t>
+  </si>
+  <si>
+    <t>Sort by</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -2427,17 +2454,8 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2457,8 +2475,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3262,10 +3289,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75D1F84-2AD1-4552-9C1F-85B59D75CCFA}">
-  <dimension ref="A1:Z167"/>
+  <dimension ref="A1:Z169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="109" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView topLeftCell="A156" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,18 +4045,18 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="83" t="s">
+      <c r="A24" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="85"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="82"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
@@ -4416,18 +4443,18 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="86" t="s">
+      <c r="A37" s="83" t="s">
         <v>172</v>
       </c>
-      <c r="B37" s="87"/>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="87"/>
-      <c r="J37" s="88"/>
+      <c r="B37" s="84"/>
+      <c r="C37" s="84"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="85"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
@@ -4846,18 +4873,18 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="86" t="s">
+      <c r="A51" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="B51" s="87"/>
-      <c r="C51" s="87"/>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="87"/>
-      <c r="H51" s="87"/>
-      <c r="I51" s="87"/>
-      <c r="J51" s="88"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="84"/>
+      <c r="I51" s="84"/>
+      <c r="J51" s="85"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="25">
@@ -5180,18 +5207,18 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="86" t="s">
+      <c r="A62" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="B62" s="87"/>
-      <c r="C62" s="87"/>
-      <c r="D62" s="87"/>
-      <c r="E62" s="87"/>
-      <c r="F62" s="87"/>
-      <c r="G62" s="87"/>
-      <c r="H62" s="87"/>
-      <c r="I62" s="87"/>
-      <c r="J62" s="88"/>
+      <c r="B62" s="84"/>
+      <c r="C62" s="84"/>
+      <c r="D62" s="84"/>
+      <c r="E62" s="84"/>
+      <c r="F62" s="84"/>
+      <c r="G62" s="84"/>
+      <c r="H62" s="84"/>
+      <c r="I62" s="84"/>
+      <c r="J62" s="85"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="25">
@@ -5546,18 +5573,18 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="86" t="s">
+      <c r="A74" s="83" t="s">
         <v>346</v>
       </c>
-      <c r="B74" s="87"/>
-      <c r="C74" s="87"/>
-      <c r="D74" s="87"/>
-      <c r="E74" s="87"/>
-      <c r="F74" s="87"/>
-      <c r="G74" s="87"/>
-      <c r="H74" s="87"/>
-      <c r="I74" s="87"/>
-      <c r="J74" s="88"/>
+      <c r="B74" s="84"/>
+      <c r="C74" s="84"/>
+      <c r="D74" s="84"/>
+      <c r="E74" s="84"/>
+      <c r="F74" s="84"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="84"/>
+      <c r="I74" s="84"/>
+      <c r="J74" s="85"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="25">
@@ -6424,18 +6451,18 @@
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="89" t="s">
+      <c r="A102" s="79" t="s">
         <v>376</v>
       </c>
-      <c r="B102" s="89"/>
-      <c r="C102" s="89"/>
-      <c r="D102" s="89"/>
-      <c r="E102" s="89"/>
-      <c r="F102" s="89"/>
-      <c r="G102" s="89"/>
-      <c r="H102" s="89"/>
-      <c r="I102" s="89"/>
-      <c r="J102" s="89"/>
+      <c r="B102" s="79"/>
+      <c r="C102" s="79"/>
+      <c r="D102" s="79"/>
+      <c r="E102" s="79"/>
+      <c r="F102" s="79"/>
+      <c r="G102" s="79"/>
+      <c r="H102" s="79"/>
+      <c r="I102" s="79"/>
+      <c r="J102" s="79"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="25">
@@ -7191,13 +7218,13 @@
       </c>
       <c r="B125" s="78"/>
       <c r="C125" s="78"/>
-      <c r="D125" s="79"/>
-      <c r="E125" s="79"/>
-      <c r="F125" s="79"/>
-      <c r="G125" s="79"/>
-      <c r="H125" s="79"/>
-      <c r="I125" s="79"/>
-      <c r="J125" s="79"/>
+      <c r="D125" s="86"/>
+      <c r="E125" s="86"/>
+      <c r="F125" s="86"/>
+      <c r="G125" s="86"/>
+      <c r="H125" s="86"/>
+      <c r="I125" s="86"/>
+      <c r="J125" s="86"/>
     </row>
     <row r="126" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="59">
@@ -7660,18 +7687,18 @@
       <c r="X135" s="58"/>
     </row>
     <row r="136" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="80" t="s">
+      <c r="A136" s="87" t="s">
         <v>442</v>
       </c>
-      <c r="B136" s="81"/>
-      <c r="C136" s="81"/>
-      <c r="D136" s="81"/>
-      <c r="E136" s="81"/>
-      <c r="F136" s="81"/>
-      <c r="G136" s="81"/>
-      <c r="H136" s="81"/>
-      <c r="I136" s="81"/>
-      <c r="J136" s="82"/>
+      <c r="B136" s="88"/>
+      <c r="C136" s="88"/>
+      <c r="D136" s="88"/>
+      <c r="E136" s="88"/>
+      <c r="F136" s="88"/>
+      <c r="G136" s="88"/>
+      <c r="H136" s="88"/>
+      <c r="I136" s="88"/>
+      <c r="J136" s="89"/>
     </row>
     <row r="137" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="25">
@@ -9043,21 +9070,68 @@
       <c r="Y167" s="58"/>
       <c r="Z167" s="58"/>
     </row>
+    <row r="168" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="78" t="s">
+        <v>605</v>
+      </c>
+      <c r="B168" s="78"/>
+      <c r="C168" s="78"/>
+      <c r="D168" s="78"/>
+      <c r="E168" s="78"/>
+      <c r="F168" s="78"/>
+      <c r="G168" s="78"/>
+      <c r="H168" s="78"/>
+      <c r="I168" s="78"/>
+      <c r="J168" s="78"/>
+    </row>
+    <row r="169" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="73">
+        <v>18</v>
+      </c>
+      <c r="B169" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C169" s="75" t="s">
+        <v>606</v>
+      </c>
+      <c r="D169" s="77" t="s">
+        <v>608</v>
+      </c>
+      <c r="E169" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="F169" s="75" t="s">
+        <v>607</v>
+      </c>
+      <c r="G169" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H169" s="74" t="s">
+        <v>544</v>
+      </c>
+      <c r="I169" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="J169" s="74" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="A168:J168"/>
     <mergeCell ref="A149:J149"/>
     <mergeCell ref="A147:J147"/>
     <mergeCell ref="A125:J125"/>
     <mergeCell ref="A136:J136"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="A115:J115"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="A102:J102"/>
     <mergeCell ref="A24:J24"/>
     <mergeCell ref="A37:J37"/>
     <mergeCell ref="A51:J51"/>
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A74:J74"/>
-    <mergeCell ref="A117:J117"/>
-    <mergeCell ref="A115:J115"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="A102:J102"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E2:J2 E8:J21 E23:J23">
@@ -9155,10 +9229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE74813B-34A6-48F5-8B35-1C10409ED694}">
-  <dimension ref="A1:U166"/>
+  <dimension ref="A1:W167"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="S162" workbookViewId="0">
+      <selection activeCell="X185" sqref="X185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9179,9 +9253,10 @@
     <col min="19" max="19" width="71.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.140625" customWidth="1"/>
     <col min="21" max="21" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>5</v>
       </c>
@@ -9245,8 +9320,14 @@
       <c r="U1" s="31" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="31" t="s">
+        <v>610</v>
+      </c>
+      <c r="W1" s="31" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>23</v>
       </c>
@@ -9306,8 +9387,14 @@
       <c r="U2" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>25</v>
       </c>
@@ -9367,8 +9454,14 @@
       <c r="U3" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W3" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>28</v>
       </c>
@@ -9428,8 +9521,14 @@
       <c r="U4" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>58</v>
       </c>
@@ -9489,8 +9588,14 @@
       <c r="U5" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W5" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>69</v>
       </c>
@@ -9550,8 +9655,14 @@
       <c r="U6" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W6" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>73</v>
       </c>
@@ -9611,8 +9722,14 @@
       <c r="U7" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="V7" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>77</v>
       </c>
@@ -9672,8 +9789,14 @@
       <c r="U8" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>79</v>
       </c>
@@ -9733,8 +9856,14 @@
       <c r="U9" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W9" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
         <v>80</v>
       </c>
@@ -9794,8 +9923,14 @@
       <c r="U10" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W10" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
         <v>81</v>
       </c>
@@ -9855,8 +9990,14 @@
       <c r="U11" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W11" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="38" t="s">
         <v>83</v>
       </c>
@@ -9916,8 +10057,14 @@
       <c r="U12" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
         <v>84</v>
       </c>
@@ -9977,8 +10124,14 @@
       <c r="U13" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W13" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
         <v>85</v>
       </c>
@@ -10038,8 +10191,14 @@
       <c r="U14" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W14" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>86</v>
       </c>
@@ -10099,8 +10258,14 @@
       <c r="U15" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
         <v>87</v>
       </c>
@@ -10160,8 +10325,14 @@
       <c r="U16" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W16" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>88</v>
       </c>
@@ -10221,8 +10392,14 @@
       <c r="U17" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W17" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>89</v>
       </c>
@@ -10282,8 +10459,14 @@
       <c r="U18" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W18" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
         <v>91</v>
       </c>
@@ -10343,8 +10526,14 @@
       <c r="U19" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W19" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>93</v>
       </c>
@@ -10404,8 +10593,14 @@
       <c r="U20" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V20" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W20" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
         <v>94</v>
       </c>
@@ -10465,8 +10660,14 @@
       <c r="U21" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V21" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
         <v>135</v>
       </c>
@@ -10526,8 +10727,14 @@
       <c r="U22" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W22" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>140</v>
       </c>
@@ -10587,8 +10794,14 @@
       <c r="U23" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W23" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>63</v>
       </c>
@@ -10648,8 +10861,14 @@
       <c r="U24" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W24" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
         <v>144</v>
       </c>
@@ -10709,8 +10928,14 @@
       <c r="U25" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W25" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
         <v>145</v>
       </c>
@@ -10770,8 +10995,14 @@
       <c r="U26" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W26" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
         <v>146</v>
       </c>
@@ -10831,8 +11062,14 @@
       <c r="U27" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W27" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
         <v>147</v>
       </c>
@@ -10892,8 +11129,14 @@
       <c r="U28" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W28" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
         <v>148</v>
       </c>
@@ -10953,8 +11196,14 @@
       <c r="U29" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W29" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
         <v>150</v>
       </c>
@@ -11014,8 +11263,14 @@
       <c r="U30" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W30" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
         <v>151</v>
       </c>
@@ -11075,8 +11330,14 @@
       <c r="U31" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V31" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W31" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
         <v>152</v>
       </c>
@@ -11136,8 +11397,14 @@
       <c r="U32" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W32" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
         <v>153</v>
       </c>
@@ -11197,8 +11464,14 @@
       <c r="U33" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V33" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W33" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
         <v>154</v>
       </c>
@@ -11258,8 +11531,14 @@
       <c r="U34" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V34" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W34" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
         <v>155</v>
       </c>
@@ -11319,8 +11598,14 @@
       <c r="U35" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V35" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W35" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>64</v>
       </c>
@@ -11380,8 +11665,14 @@
       <c r="U36" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V36" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W36" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
         <v>175</v>
       </c>
@@ -11443,8 +11734,14 @@
       <c r="U37" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W37" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
         <v>179</v>
       </c>
@@ -11506,8 +11803,14 @@
       <c r="U38" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V38" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W38" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
         <v>182</v>
       </c>
@@ -11569,8 +11872,14 @@
       <c r="U39" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V39" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W39" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
         <v>185</v>
       </c>
@@ -11632,8 +11941,14 @@
       <c r="U40" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V40" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W40" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="47" t="s">
         <v>188</v>
       </c>
@@ -11695,8 +12010,14 @@
       <c r="U41" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V41" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W41" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
         <v>190</v>
       </c>
@@ -11758,8 +12079,14 @@
       <c r="U42" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V42" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W42" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
         <v>193</v>
       </c>
@@ -11821,8 +12148,14 @@
       <c r="U43" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V43" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W43" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
         <v>196</v>
       </c>
@@ -11884,8 +12217,14 @@
       <c r="U44" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V44" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W44" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
         <v>199</v>
       </c>
@@ -11947,8 +12286,14 @@
       <c r="U45" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V45" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W45" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
         <v>201</v>
       </c>
@@ -12010,8 +12355,14 @@
       <c r="U46" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V46" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W46" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="47" t="s">
         <v>203</v>
       </c>
@@ -12073,8 +12424,14 @@
       <c r="U47" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V47" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W47" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" s="47" t="s">
         <v>205</v>
       </c>
@@ -12136,8 +12493,14 @@
       <c r="U48" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V48" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W48" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
         <v>207</v>
       </c>
@@ -12199,8 +12562,14 @@
       <c r="U49" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V49" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W49" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
         <v>209</v>
       </c>
@@ -12262,8 +12631,14 @@
       <c r="U50" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V50" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W50" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
         <v>211</v>
       </c>
@@ -12325,8 +12700,14 @@
       <c r="U51" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V51" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W51" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" s="47" t="s">
         <v>213</v>
       </c>
@@ -12388,8 +12769,14 @@
       <c r="U52" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V52" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W52" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" s="55" t="s">
         <v>214</v>
       </c>
@@ -12451,8 +12838,14 @@
       <c r="U53" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V53" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W53" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" s="48" t="s">
         <v>215</v>
       </c>
@@ -12514,8 +12907,14 @@
       <c r="U54" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V54" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W54" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" s="48" t="s">
         <v>216</v>
       </c>
@@ -12577,8 +12976,14 @@
       <c r="U55" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V55" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W55" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" s="48" t="s">
         <v>217</v>
       </c>
@@ -12640,8 +13045,14 @@
       <c r="U56" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V56" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W56" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" s="48" t="s">
         <v>218</v>
       </c>
@@ -12703,8 +13114,14 @@
       <c r="U57" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V57" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W57" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="48" t="s">
         <v>219</v>
       </c>
@@ -12766,8 +13183,14 @@
       <c r="U58" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V58" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W58" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="48" t="s">
         <v>220</v>
       </c>
@@ -12829,8 +13252,14 @@
       <c r="U59" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V59" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W59" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="48" t="s">
         <v>221</v>
       </c>
@@ -12892,8 +13321,14 @@
       <c r="U60" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V60" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W60" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61" s="48" t="s">
         <v>222</v>
       </c>
@@ -12955,8 +13390,14 @@
       <c r="U61" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V61" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W61" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" s="51" t="s">
         <v>223</v>
       </c>
@@ -13018,8 +13459,14 @@
       <c r="U62" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V62" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W62" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" s="56" t="s">
         <v>250</v>
       </c>
@@ -13081,8 +13528,14 @@
       <c r="U63" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V63" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W63" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" s="48" t="s">
         <v>254</v>
       </c>
@@ -13144,8 +13597,14 @@
       <c r="U64" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V64" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W64" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" s="48" t="s">
         <v>257</v>
       </c>
@@ -13207,8 +13666,14 @@
       <c r="U65" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V65" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W65" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" s="48" t="s">
         <v>260</v>
       </c>
@@ -13270,8 +13735,14 @@
       <c r="U66" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V66" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W66" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67" s="48" t="s">
         <v>263</v>
       </c>
@@ -13333,8 +13804,14 @@
       <c r="U67" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V67" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W67" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" s="48" t="s">
         <v>266</v>
       </c>
@@ -13396,8 +13873,14 @@
       <c r="U68" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V68" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W68" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69" s="48" t="s">
         <v>269</v>
       </c>
@@ -13459,8 +13942,14 @@
       <c r="U69" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V69" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W69" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" s="48" t="s">
         <v>272</v>
       </c>
@@ -13522,8 +14011,14 @@
       <c r="U70" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V70" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W70" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
         <v>275</v>
       </c>
@@ -13585,8 +14080,14 @@
       <c r="U71" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V71" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W71" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
         <v>278</v>
       </c>
@@ -13648,8 +14149,14 @@
       <c r="U72" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V72" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W72" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" s="51" t="s">
         <v>281</v>
       </c>
@@ -13713,8 +14220,14 @@
       <c r="U73" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V73" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W73" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" s="62" t="s">
         <v>283</v>
       </c>
@@ -13778,8 +14291,14 @@
       <c r="U74" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V74" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W74" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
         <v>286</v>
       </c>
@@ -13843,8 +14362,14 @@
       <c r="U75" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V75" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W75" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
         <v>288</v>
       </c>
@@ -13908,8 +14433,14 @@
       <c r="U76" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V76" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W76" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
         <v>290</v>
       </c>
@@ -13973,8 +14504,14 @@
       <c r="U77" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V77" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W77" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" s="48" t="s">
         <v>293</v>
       </c>
@@ -14038,8 +14575,14 @@
       <c r="U78" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V78" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W78" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" s="48" t="s">
         <v>296</v>
       </c>
@@ -14103,8 +14646,14 @@
       <c r="U79" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V79" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W79" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" s="48" t="s">
         <v>299</v>
       </c>
@@ -14168,8 +14717,14 @@
       <c r="U80" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V80" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W80" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="48" t="s">
         <v>302</v>
       </c>
@@ -14233,8 +14788,14 @@
       <c r="U81" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V81" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W81" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="48" t="s">
         <v>305</v>
       </c>
@@ -14298,8 +14859,14 @@
       <c r="U82" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V82" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W82" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="48" t="s">
         <v>307</v>
       </c>
@@ -14363,8 +14930,14 @@
       <c r="U83" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V83" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W83" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="48" t="s">
         <v>309</v>
       </c>
@@ -14428,8 +15001,14 @@
       <c r="U84" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V84" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W84" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
         <v>311</v>
       </c>
@@ -14493,8 +15072,14 @@
       <c r="U85" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V85" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W85" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="48" t="s">
         <v>314</v>
       </c>
@@ -14558,8 +15143,14 @@
       <c r="U86" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V86" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W86" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="48" t="s">
         <v>317</v>
       </c>
@@ -14623,8 +15214,14 @@
       <c r="U87" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V87" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W87" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="48" t="s">
         <v>320</v>
       </c>
@@ -14688,8 +15285,14 @@
       <c r="U88" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V88" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W88" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="48" t="s">
         <v>323</v>
       </c>
@@ -14753,8 +15356,14 @@
       <c r="U89" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V89" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W89" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="48" t="s">
         <v>325</v>
       </c>
@@ -14818,8 +15427,14 @@
       <c r="U90" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V90" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W90" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" s="48" t="s">
         <v>328</v>
       </c>
@@ -14883,8 +15498,14 @@
       <c r="U91" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V91" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W91" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="48" t="s">
         <v>331</v>
       </c>
@@ -14948,8 +15569,14 @@
       <c r="U92" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V92" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W92" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" s="48" t="s">
         <v>333</v>
       </c>
@@ -15013,8 +15640,14 @@
       <c r="U93" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V93" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W93" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="48" t="s">
         <v>335</v>
       </c>
@@ -15078,8 +15711,14 @@
       <c r="U94" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V94" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W94" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" s="48" t="s">
         <v>337</v>
       </c>
@@ -15143,8 +15782,14 @@
       <c r="U95" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V95" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W95" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="48" t="s">
         <v>339</v>
       </c>
@@ -15208,8 +15853,14 @@
       <c r="U96" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V96" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W96" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97" s="48" t="s">
         <v>341</v>
       </c>
@@ -15273,8 +15924,14 @@
       <c r="U97" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V97" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W97" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98" s="48" t="s">
         <v>343</v>
       </c>
@@ -15338,8 +15995,14 @@
       <c r="U98" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V98" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W98" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99" s="48" t="s">
         <v>345</v>
       </c>
@@ -15403,8 +16066,14 @@
       <c r="U99" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V99" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W99" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100" s="48" t="s">
         <v>601</v>
       </c>
@@ -15468,8 +16137,14 @@
       <c r="U100" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V100" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W100" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101" s="48" t="s">
         <v>349</v>
       </c>
@@ -15533,8 +16208,14 @@
       <c r="U101" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V101" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W101" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102" s="48" t="s">
         <v>353</v>
       </c>
@@ -15598,8 +16279,14 @@
       <c r="U102" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V102" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W102" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" s="48" t="s">
         <v>356</v>
       </c>
@@ -15663,8 +16350,14 @@
       <c r="U103" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V103" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W103" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104" s="48" t="s">
         <v>359</v>
       </c>
@@ -15728,8 +16421,14 @@
       <c r="U104" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V104" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W104" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" s="48" t="s">
         <v>362</v>
       </c>
@@ -15793,8 +16492,14 @@
       <c r="U105" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V105" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W105" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106" s="48" t="s">
         <v>365</v>
       </c>
@@ -15858,8 +16563,14 @@
       <c r="U106" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V106" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W106" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107" s="48" t="s">
         <v>368</v>
       </c>
@@ -15923,8 +16634,14 @@
       <c r="U107" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V107" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W107" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108" s="48" t="s">
         <v>370</v>
       </c>
@@ -15988,8 +16705,14 @@
       <c r="U108" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V108" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W108" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" s="48" t="s">
         <v>372</v>
       </c>
@@ -16053,8 +16776,14 @@
       <c r="U109" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V109" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W109" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110" s="48" t="s">
         <v>602</v>
       </c>
@@ -16118,8 +16847,14 @@
       <c r="U110" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V110" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W110" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111" s="48" t="s">
         <v>380</v>
       </c>
@@ -16183,8 +16918,14 @@
       <c r="U111" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V111" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W111" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" s="48" t="s">
         <v>385</v>
       </c>
@@ -16248,8 +16989,14 @@
       <c r="U112" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V112" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W112" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113" s="48" t="s">
         <v>399</v>
       </c>
@@ -16313,8 +17060,14 @@
       <c r="U113" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V113" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W113" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114" s="48" t="s">
         <v>401</v>
       </c>
@@ -16378,8 +17131,14 @@
       <c r="U114" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V114" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W114" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115" s="48" t="s">
         <v>402</v>
       </c>
@@ -16443,8 +17202,14 @@
       <c r="U115" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V115" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W115" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116" s="48" t="s">
         <v>403</v>
       </c>
@@ -16508,8 +17273,14 @@
       <c r="U116" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V116" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W116" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117" s="48" t="s">
         <v>404</v>
       </c>
@@ -16573,8 +17344,14 @@
       <c r="U117" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V117" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W117" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118" s="48" t="s">
         <v>405</v>
       </c>
@@ -16638,8 +17415,14 @@
       <c r="U118" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V118" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W118" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" s="48" t="s">
         <v>407</v>
       </c>
@@ -16703,8 +17486,14 @@
       <c r="U119" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V119" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W119" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" s="48" t="s">
         <v>409</v>
       </c>
@@ -16768,8 +17557,14 @@
       <c r="U120" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="121" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="V120" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W120" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A121" s="62" t="s">
         <v>415</v>
       </c>
@@ -16833,8 +17628,14 @@
       <c r="U121" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V121" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W121" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122" s="48" t="s">
         <v>419</v>
       </c>
@@ -16898,8 +17699,14 @@
       <c r="U122" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V122" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W122" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123" s="48" t="s">
         <v>422</v>
       </c>
@@ -16963,8 +17770,14 @@
       <c r="U123" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="124" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="V123" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W123" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A124" s="48" t="s">
         <v>424</v>
       </c>
@@ -17028,8 +17841,14 @@
       <c r="U124" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="125" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="V124" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W124" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A125" s="48" t="s">
         <v>426</v>
       </c>
@@ -17093,8 +17912,14 @@
       <c r="U125" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V125" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W125" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" s="48" t="s">
         <v>429</v>
       </c>
@@ -17158,8 +17983,14 @@
       <c r="U126" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V126" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W126" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127" s="48" t="s">
         <v>432</v>
       </c>
@@ -17223,8 +18054,14 @@
       <c r="U127" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V127" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W127" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128" s="48" t="s">
         <v>435</v>
       </c>
@@ -17288,8 +18125,14 @@
       <c r="U128" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="129" spans="1:21" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="V128" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W128" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A129" s="48" t="s">
         <v>438</v>
       </c>
@@ -17353,8 +18196,14 @@
       <c r="U129" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V129" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W129" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A130" s="48" t="s">
         <v>441</v>
       </c>
@@ -17418,8 +18267,14 @@
       <c r="U130" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V130" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W130" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A131" s="48" t="s">
         <v>399</v>
       </c>
@@ -17483,8 +18338,14 @@
       <c r="U131" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V131" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W131" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A132" s="48" t="s">
         <v>401</v>
       </c>
@@ -17548,8 +18409,14 @@
       <c r="U132" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V132" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W132" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A133" s="48" t="s">
         <v>402</v>
       </c>
@@ -17613,8 +18480,14 @@
       <c r="U133" s="48" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V133" s="48" t="s">
+        <v>493</v>
+      </c>
+      <c r="W133" s="48" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A134" s="48" t="s">
         <v>403</v>
       </c>
@@ -17678,8 +18551,14 @@
       <c r="U134" s="48" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V134" s="48" t="s">
+        <v>487</v>
+      </c>
+      <c r="W134" s="48" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A135" s="48" t="s">
         <v>404</v>
       </c>
@@ -17743,8 +18622,14 @@
       <c r="U135" s="48" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V135" s="48" t="s">
+        <v>488</v>
+      </c>
+      <c r="W135" s="48" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A136" s="48" t="s">
         <v>405</v>
       </c>
@@ -17808,8 +18693,14 @@
       <c r="U136" s="48" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V136" s="48" t="s">
+        <v>489</v>
+      </c>
+      <c r="W136" s="48" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A137" s="48" t="s">
         <v>407</v>
       </c>
@@ -17873,8 +18764,14 @@
       <c r="U137" s="48" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V137" s="48" t="s">
+        <v>490</v>
+      </c>
+      <c r="W137" s="48" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A138" s="48" t="s">
         <v>445</v>
       </c>
@@ -17938,8 +18835,14 @@
       <c r="U138" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V138" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W138" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A139" s="48" t="s">
         <v>449</v>
       </c>
@@ -18003,8 +18906,14 @@
       <c r="U139" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V139" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W139" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A140" s="48" t="s">
         <v>452</v>
       </c>
@@ -18068,8 +18977,14 @@
       <c r="U140" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V140" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W140" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A141" s="48" t="s">
         <v>454</v>
       </c>
@@ -18133,8 +19048,14 @@
       <c r="U141" s="48" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V141" s="48" t="s">
+        <v>535</v>
+      </c>
+      <c r="W141" s="48" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A142" s="48" t="s">
         <v>457</v>
       </c>
@@ -18198,8 +19119,14 @@
       <c r="U142" s="48" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V142" s="48" t="s">
+        <v>487</v>
+      </c>
+      <c r="W142" s="48" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A143" s="48" t="s">
         <v>460</v>
       </c>
@@ -18263,8 +19190,14 @@
       <c r="U143" s="48" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V143" s="48" t="s">
+        <v>488</v>
+      </c>
+      <c r="W143" s="48" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A144" s="48" t="s">
         <v>463</v>
       </c>
@@ -18328,8 +19261,14 @@
       <c r="U144" s="48" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V144" s="48" t="s">
+        <v>489</v>
+      </c>
+      <c r="W144" s="48" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A145" s="48" t="s">
         <v>466</v>
       </c>
@@ -18393,8 +19332,14 @@
       <c r="U145" s="48" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="146" spans="1:21" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="V145" s="48" t="s">
+        <v>490</v>
+      </c>
+      <c r="W145" s="48" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="146" spans="1:23" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A146" s="48" t="s">
         <v>469</v>
       </c>
@@ -18458,8 +19403,14 @@
       <c r="U146" s="48" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="147" spans="1:21" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="V146" s="48" t="s">
+        <v>491</v>
+      </c>
+      <c r="W146" s="48" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="147" spans="1:23" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A147" s="48" t="s">
         <v>472</v>
       </c>
@@ -18523,8 +19474,14 @@
       <c r="U147" s="48" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="148" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V147" s="48" t="s">
+        <v>492</v>
+      </c>
+      <c r="W147" s="48" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="148" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="48" t="s">
         <v>513</v>
       </c>
@@ -18588,8 +19545,14 @@
       <c r="U148" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="149" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V148" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W148" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="149" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="67" t="s">
         <v>543</v>
       </c>
@@ -18653,8 +19616,14 @@
       <c r="U149" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="150" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V149" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W149" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="150" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="70" t="s">
         <v>547</v>
       </c>
@@ -18718,8 +19687,14 @@
       <c r="U150" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="151" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V150" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W150" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="151" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="67" t="s">
         <v>550</v>
       </c>
@@ -18783,8 +19758,14 @@
       <c r="U151" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="152" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V151" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W151" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="152" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="70" t="s">
         <v>553</v>
       </c>
@@ -18848,8 +19829,14 @@
       <c r="U152" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="153" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V152" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W152" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="153" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="67" t="s">
         <v>555</v>
       </c>
@@ -18913,8 +19900,14 @@
       <c r="U153" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="154" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V153" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W153" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="154" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="70" t="s">
         <v>557</v>
       </c>
@@ -18978,8 +19971,14 @@
       <c r="U154" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="155" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V154" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W154" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="67" t="s">
         <v>559</v>
       </c>
@@ -19043,8 +20042,14 @@
       <c r="U155" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="156" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V155" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W155" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="156" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="70" t="s">
         <v>561</v>
       </c>
@@ -19108,8 +20113,14 @@
       <c r="U156" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="157" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V156" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W156" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="157" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="67" t="s">
         <v>563</v>
       </c>
@@ -19173,8 +20184,14 @@
       <c r="U157" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="158" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V157" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W157" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="158" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="70" t="s">
         <v>566</v>
       </c>
@@ -19238,8 +20255,14 @@
       <c r="U158" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="159" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V158" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W158" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="67" t="s">
         <v>569</v>
       </c>
@@ -19303,8 +20326,14 @@
       <c r="U159" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="160" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V159" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W159" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="70" t="s">
         <v>572</v>
       </c>
@@ -19368,8 +20397,14 @@
       <c r="U160" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="161" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V160" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W160" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="161" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="67" t="s">
         <v>575</v>
       </c>
@@ -19433,8 +20468,14 @@
       <c r="U161" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="162" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V161" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W161" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="70" t="s">
         <v>578</v>
       </c>
@@ -19498,8 +20539,14 @@
       <c r="U162" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="163" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V162" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W162" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="67" t="s">
         <v>581</v>
       </c>
@@ -19563,8 +20610,14 @@
       <c r="U163" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="164" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V163" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W163" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="164" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="67" t="s">
         <v>583</v>
       </c>
@@ -19628,8 +20681,14 @@
       <c r="U164" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="165" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V164" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W164" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="165" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="67" t="s">
         <v>585</v>
       </c>
@@ -19693,8 +20752,14 @@
       <c r="U165" s="48" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="166" spans="1:21" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V165" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W165" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="67" t="s">
         <v>588</v>
       </c>
@@ -19757,6 +20822,83 @@
       </c>
       <c r="U166" s="48" t="s">
         <v>22</v>
+      </c>
+      <c r="V166" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="W166" s="48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="75" t="s">
+        <v>607</v>
+      </c>
+      <c r="B167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="J167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="K167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="L167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="M167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="N167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="O167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="R167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="S167" s="49" t="s">
+        <v>609</v>
+      </c>
+      <c r="T167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="U167" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="V167" s="48" t="s">
+        <v>611</v>
+      </c>
+      <c r="W167" s="36" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -19883,8 +21025,9 @@
     <hyperlink ref="G126" r:id="rId15" xr:uid="{FEC9AB2B-6FD0-4D08-96BB-5634F117BFB0}"/>
     <hyperlink ref="D136" r:id="rId16" xr:uid="{EAE526E7-10C0-4EC9-846A-D81343ACBEC4}"/>
     <hyperlink ref="G166" r:id="rId17" xr:uid="{0A52F660-ABF2-41CF-BD4C-5E55458D590D}"/>
+    <hyperlink ref="S167" r:id="rId18" xr:uid="{13FB8A07-5562-4AAB-9E83-934C01965617}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>